<commit_message>
Adding screenshot and Allure reports
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata.xlsx
+++ b/src/test/resources/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation\New_Folder\AutomationSauceLab\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA27918F-3009-4B99-891D-3CEFEC79F4FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A724A01-AE49-43A5-8220-08ACEA6DFC10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{11F41CD3-5DDB-45E0-925E-D744450FF265}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
   <si>
     <t>standard_user</t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t>Epic sadface: Password is required</t>
+  </si>
+  <si>
+    <t>Epic sadface: Username and password do not match any user in this service1</t>
   </si>
 </sst>
 </file>
@@ -441,7 +444,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -457,7 +460,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
Add Remote webdriver option to execute the tests
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata.xlsx
+++ b/src/test/resources/testdata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation\New_Folder\AutomationSauceLab\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A724A01-AE49-43A5-8220-08ACEA6DFC10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DE36266-7083-434A-AFF4-719CFE548C8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{11F41CD3-5DDB-45E0-925E-D744450FF265}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="8">
   <si>
     <t>standard_user</t>
   </si>
@@ -60,9 +60,6 @@
   </si>
   <si>
     <t>Epic sadface: Password is required</t>
-  </si>
-  <si>
-    <t>Epic sadface: Username and password do not match any user in this service1</t>
   </si>
 </sst>
 </file>
@@ -460,7 +457,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>

</xml_diff>